<commit_message>
Saving future me from having wrong packages at assembly
</commit_message>
<xml_diff>
--- a/hardware/radio_module/rev_b/radio_module_bom.xlsx
+++ b/hardware/radio_module/rev_b/radio_module_bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="284">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -163,7 +163,7 @@
     <t xml:space="preserve">FB1</t>
   </si>
   <si>
-    <t xml:space="preserve">490-5216-1-ND</t>
+    <t xml:space="preserve">445-2158-1-ND</t>
   </si>
   <si>
     <t xml:space="preserve">R7, R8, R9</t>
@@ -475,33 +475,36 @@
     <t xml:space="preserve">C8</t>
   </si>
   <si>
+    <t xml:space="preserve">712-1342-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C31, C32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-13252-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-3254-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10, C11, C12</t>
+  </si>
+  <si>
     <t xml:space="preserve">490-6241-1-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">4.7uF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C31, C32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-13252-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47nF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-3254-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47pF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C10, C11, C12</t>
-  </si>
-  <si>
     <t xml:space="preserve">C9</t>
   </si>
   <si>
@@ -685,7 +688,7 @@
     <t xml:space="preserve">Generic NMOS footprint</t>
   </si>
   <si>
-    <t xml:space="preserve">SI2333DDS-T1-GE3CT-ND </t>
+    <t xml:space="preserve">2N7002LT1GOSCT-ND</t>
   </si>
   <si>
     <t xml:space="preserve">NANO_SIM</t>
@@ -883,6 +886,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -942,9 +946,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -966,30 +974,30 @@
   </sheetPr>
   <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A60" activeCellId="0" sqref="A60"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F17" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.21428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.0255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="60.6377551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="71.1428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9285714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8163265306122"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.20918367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.0204081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.71428571428571"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.21938775510204"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.0255102040816"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.219387755102"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.41326530612245"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="22.1224489795918"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="19.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.35714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="33.515306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.9438775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64.1938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="75.3265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.4489795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2244897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.5612244897959"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.46938775510204"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.9081632653061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.08163265306122"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.1581632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.92857142857143"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="23.3877551020408"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="12.1479591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1939,7 +1947,7 @@
         <v>42</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1956,13 +1964,13 @@
         <v>40</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F41" s="0" t="s">
         <v>42</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1970,7 +1978,7 @@
         <v>1</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>39</v>
@@ -1979,13 +1987,13 @@
         <v>40</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>42</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1993,7 +2001,7 @@
         <v>2</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>27</v>
@@ -2002,13 +2010,13 @@
         <v>28</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F43" s="0" t="s">
         <v>30</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2016,7 +2024,7 @@
         <v>2</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>39</v>
@@ -2025,13 +2033,13 @@
         <v>40</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>42</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2039,28 +2047,28 @@
         <v>1</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D45" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="K45" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="N45" s="0" t="s">
         <v>172</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="G45" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="K45" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="N45" s="0" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2068,28 +2076,28 @@
         <v>1</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E46" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="K46" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="N46" s="0" t="s">
         <v>178</v>
-      </c>
-      <c r="F46" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="G46" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="K46" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="N46" s="0" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2097,25 +2105,25 @@
         <v>1</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="Q47" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2123,22 +2131,22 @@
         <v>3</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2146,22 +2154,22 @@
         <v>1</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="R49" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2169,22 +2177,22 @@
         <v>3</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2192,34 +2200,34 @@
         <v>1</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="L51" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="M51" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O51" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="P51" s="0" t="n">
         <v>15912080</v>
@@ -2230,25 +2238,25 @@
         <v>2</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K52" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="N52" s="0" t="n">
         <v>732511350</v>
@@ -2259,22 +2267,22 @@
         <v>3</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="G53" s="0" t="s">
         <v>221</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2282,22 +2290,22 @@
         <v>1</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2305,25 +2313,25 @@
         <v>1</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="Q55" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2331,22 +2339,22 @@
         <v>1</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2354,22 +2362,22 @@
         <v>1</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2377,22 +2385,22 @@
         <v>3</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2400,22 +2408,22 @@
         <v>1</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2423,22 +2431,22 @@
         <v>4</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2446,28 +2454,28 @@
         <v>2</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="K61" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="N61" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,22 +2483,22 @@
         <v>1</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2498,28 +2506,28 @@
         <v>2</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="K63" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="N63" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2527,19 +2535,19 @@
         <v>1</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2547,19 +2555,19 @@
         <v>1</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>